<commit_message>
Fix final pre entrega
</commit_message>
<xml_diff>
--- a/wwwroot/files/ExcelModeloRecuento4.xlsx
+++ b/wwwroot/files/ExcelModeloRecuento4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaston Michelotti\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaston Michelotti\source\repos\intelmec\wwwroot\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{025EA4AB-C678-4CC8-A067-98BF99E69CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE50F6E9-113B-4180-A0B0-6DE2222D917B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3536,16 +3536,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E1029"/>
+    <sheetView tabSelected="1" topLeftCell="A956" workbookViewId="0">
+      <selection activeCell="D974" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="30.7265625" style="2"/>
     <col min="3" max="3" width="36.81640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" style="5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="16384" width="30.7265625" style="2"/>
   </cols>
   <sheetData>

</xml_diff>